<commit_message>
start of report template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
+++ b/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A904131-A05D-2046-AA4C-BFEF619C40DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29157E4E-3BB2-314D-93F3-0C600DBCF3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26700" yWindow="2500" windowWidth="34840" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Multi-Year Historical Project Recovery Information</t>
   </si>
   <si>
-    <t>For Fiscal Years {fiscal_year1} to {fiscal_year2}</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>{quarter_multi_year_q4_grand_total}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Fiscal Years {d.reportFiscalYears.fiscalFrom} to {d.reportFiscalYears.fiscalTo} </t>
   </si>
 </sst>
 </file>
@@ -244,9 +244,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,10 +257,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -275,6 +269,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,358 +656,358 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="8.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="13" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="29" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="29" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="25" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10"/>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="12"/>
-      <c r="B6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="C8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="10"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added combination of total by fiscal
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
+++ b/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29157E4E-3BB2-314D-93F3-0C600DBCF3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA97B00C-E6B8-C84E-BECB-8B4D88A61B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Project Name</t>
   </si>
@@ -62,77 +62,89 @@
     <t>Quarter 4</t>
   </si>
   <si>
-    <t>{project_number}</t>
-  </si>
-  <si>
-    <t>{project_name}</t>
-  </si>
-  <si>
-    <t>{quarter1_amount}</t>
-  </si>
-  <si>
-    <t>{quarter2_amount}</t>
-  </si>
-  <si>
-    <t>{quarter3_amount}</t>
-  </si>
-  <si>
-    <t>{quarter4_amount}</t>
-  </si>
-  <si>
-    <t>{quarter_total}</t>
-  </si>
-  <si>
-    <t>{quarter_grand_total}</t>
-  </si>
-  <si>
-    <t>{quarter1_grandTotal_amount}</t>
-  </si>
-  <si>
-    <t>{quarter2_grandTotal_amount}</t>
-  </si>
-  <si>
-    <t>{quarter3_grandTotal_amount}</t>
-  </si>
-  <si>
-    <t>{quarter4_grandTotal_amount}</t>
-  </si>
-  <si>
     <t>Fiscal Totals</t>
   </si>
   <si>
-    <t>Recoveries for FY:  {fiscal[i]}</t>
-  </si>
-  <si>
-    <t>fiscal[i+1]</t>
-  </si>
-  <si>
     <t>Multi-Fiscal Total</t>
   </si>
   <si>
-    <t>{quarter_multi_year_grand_total}</t>
-  </si>
-  <si>
-    <t>{quarter_multi_year_q1_grand_total}</t>
-  </si>
-  <si>
-    <t>{quarter_multi_year_q2_grand_total}</t>
-  </si>
-  <si>
-    <t>{quarter_multi_year_q3_grand_total}</t>
-  </si>
-  <si>
-    <t>{quarter_multi_year_q4_grand_total}</t>
-  </si>
-  <si>
     <t xml:space="preserve">For Fiscal Years {d.reportFiscalYears.fiscalFrom} to {d.reportFiscalYears.fiscalTo} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recoveries for FY:  </t>
+  </si>
+  <si>
+    <t>{#rptRecov=d.reportRecoveriesWithTotals[i].sectionInfo[i]}</t>
+  </si>
+  <si>
+    <t>{#rptRecov1=d.reportRecoveriesWithTotals[i].sectionInfo[i+1]}</t>
+  </si>
+  <si>
+    <t>{#rptRecovGrand1=d.reportRecoveriesWithTotals[i+1].sectionTotals}</t>
+  </si>
+  <si>
+    <t>{#rptRecovGrand=d.reportRecoveriesWithTotals[i].sectionTotals}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.project_name}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.q1}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.q2}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.q3}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.q4}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.total_recovered}</t>
+  </si>
+  <si>
+    <t>{$rptRecov1}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand.q1}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand.q2}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand.q3}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand.q4}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand.recovered_total}</t>
+  </si>
+  <si>
+    <t>{$rptRecovGrand1}</t>
+  </si>
+  <si>
+    <t>{$rptRecov.project_number}</t>
+  </si>
+  <si>
+    <t>{#rptRecovFiscal=d.reportRecoveriesWithTotals[i].sectionFiscal}</t>
+  </si>
+  <si>
+    <t>{$rptRecovFiscal}</t>
+  </si>
+  <si>
+    <t>{#rptRecovFiscal1=d.reportRecoveriesWithTotals[i+1].sectionFiscal}</t>
+  </si>
+  <si>
+    <t>{$rptRecovFiscal1}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +188,11 @@
       <color theme="1"/>
       <name val="BC Sans Regular"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -203,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -235,11 +252,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -250,18 +280,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -269,12 +292,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,7 +349,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1327313</xdr:colOff>
+      <xdr:colOff>740338</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>153695</xdr:rowOff>
     </xdr:to>
@@ -653,51 +693,52 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="10" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="29" customHeight="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="29" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" ht="25" customHeight="1">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="25" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="C2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -716,304 +757,332 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8"/>
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="10"/>
-      <c r="B6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="10"/>
-      <c r="B8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="10"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>